<commit_message>
update some marks in excel
</commit_message>
<xml_diff>
--- a/docs/smtcomp25_stats.xlsx
+++ b/docs/smtcomp25_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengyanglu/Desktop/z3alpha/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2A9B09-6EC1-D04F-AA53-07CE9B3AC670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FADC08-59AF-C342-B97A-9589EB728896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38000" yWindow="-680" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-680" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Division_summuary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>Logics</t>
   </si>
@@ -162,13 +162,46 @@
   </si>
   <si>
     <t>Z3</t>
+  </si>
+  <si>
+    <t>434 [1 core]</t>
+  </si>
+  <si>
+    <t>2200 [1 core]</t>
+  </si>
+  <si>
+    <t>114 [1 core, strategy to be updated]</t>
+  </si>
+  <si>
+    <t>38 [1 core]</t>
+  </si>
+  <si>
+    <t>1267 [1 core]</t>
+  </si>
+  <si>
+    <t>0 [1 core]</t>
+  </si>
+  <si>
+    <t>1023 [1 core]</t>
+  </si>
+  <si>
+    <t>978 [1 core]</t>
+  </si>
+  <si>
+    <t>3949 [1 core]</t>
+  </si>
+  <si>
+    <t>1942 [1 core]</t>
+  </si>
+  <si>
+    <t>19201 [1 core]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -203,6 +236,11 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="7">
@@ -456,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -609,23 +647,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1115,7 +1162,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1124,7 +1171,8 @@
     <col min="2" max="2" width="22.6640625" style="8" customWidth="1"/>
     <col min="3" max="3" width="24.5" style="9" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" style="9" customWidth="1"/>
-    <col min="5" max="6" width="24.83203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="39" style="9" customWidth="1"/>
     <col min="7" max="7" width="91.5" style="10" customWidth="1"/>
     <col min="8" max="8" width="62.6640625" style="10" customWidth="1"/>
   </cols>
@@ -1154,7 +1202,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="54" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -1167,14 +1215,14 @@
       <c r="E2" s="18">
         <v>387</v>
       </c>
-      <c r="F2" s="18">
-        <v>434</v>
+      <c r="F2" s="60" t="s">
+        <v>43</v>
       </c>
       <c r="G2" s="32"/>
-      <c r="H2" s="56"/>
+      <c r="H2" s="59"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="58"/>
+      <c r="A3" s="54"/>
       <c r="B3" s="19" t="s">
         <v>9</v>
       </c>
@@ -1185,14 +1233,14 @@
       <c r="E3" s="20">
         <v>2177</v>
       </c>
-      <c r="F3" s="20">
-        <v>2200</v>
+      <c r="F3" s="61" t="s">
+        <v>44</v>
       </c>
       <c r="G3" s="33"/>
-      <c r="H3" s="56"/>
+      <c r="H3" s="59"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="58"/>
+      <c r="A4" s="54"/>
       <c r="B4" s="19" t="s">
         <v>10</v>
       </c>
@@ -1205,14 +1253,14 @@
       <c r="E4" s="20">
         <v>210</v>
       </c>
-      <c r="F4" s="20">
-        <v>114</v>
+      <c r="F4" s="61" t="s">
+        <v>45</v>
       </c>
       <c r="G4" s="33"/>
-      <c r="H4" s="56"/>
+      <c r="H4" s="59"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="21" t="s">
         <v>12</v>
       </c>
@@ -1225,7 +1273,7 @@
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="34"/>
-      <c r="H5" s="56"/>
+      <c r="H5" s="59"/>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
@@ -1248,7 +1296,7 @@
       <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="55" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -1259,14 +1307,14 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
-      <c r="F7" s="18">
-        <v>38</v>
+      <c r="F7" s="60" t="s">
+        <v>46</v>
       </c>
       <c r="G7" s="32"/>
-      <c r="H7" s="56"/>
+      <c r="H7" s="59"/>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="59"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="19" t="s">
         <v>17</v>
       </c>
@@ -1277,14 +1325,14 @@
       <c r="E8" s="20">
         <v>1265</v>
       </c>
-      <c r="F8" s="20">
-        <v>1267</v>
+      <c r="F8" s="61" t="s">
+        <v>47</v>
       </c>
       <c r="G8" s="33"/>
-      <c r="H8" s="56"/>
+      <c r="H8" s="59"/>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="59"/>
+      <c r="A9" s="55"/>
       <c r="B9" s="19" t="s">
         <v>18</v>
       </c>
@@ -1293,14 +1341,14 @@
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="20">
-        <v>0</v>
+      <c r="F9" s="61" t="s">
+        <v>48</v>
       </c>
       <c r="G9" s="33"/>
-      <c r="H9" s="56"/>
+      <c r="H9" s="59"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="59"/>
+      <c r="A10" s="55"/>
       <c r="B10" s="19" t="s">
         <v>19</v>
       </c>
@@ -1311,14 +1359,14 @@
       <c r="E10" s="20">
         <v>1029</v>
       </c>
-      <c r="F10" s="20">
-        <v>1023</v>
+      <c r="F10" s="61" t="s">
+        <v>49</v>
       </c>
       <c r="G10" s="33"/>
-      <c r="H10" s="56"/>
+      <c r="H10" s="59"/>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="59"/>
+      <c r="A11" s="55"/>
       <c r="B11" s="19" t="s">
         <v>20</v>
       </c>
@@ -1327,14 +1375,14 @@
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="20">
-        <v>978</v>
+      <c r="F11" s="61" t="s">
+        <v>50</v>
       </c>
       <c r="G11" s="33"/>
-      <c r="H11" s="56"/>
+      <c r="H11" s="59"/>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="59"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="19" t="s">
         <v>21</v>
       </c>
@@ -1345,14 +1393,14 @@
       <c r="E12" s="20">
         <v>3935</v>
       </c>
-      <c r="F12" s="20">
-        <v>3949</v>
+      <c r="F12" s="61" t="s">
+        <v>51</v>
       </c>
       <c r="G12" s="33"/>
-      <c r="H12" s="56"/>
+      <c r="H12" s="59"/>
     </row>
     <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="31" t="s">
         <v>22</v>
       </c>
@@ -1365,7 +1413,7 @@
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="34"/>
-      <c r="H13" s="56"/>
+      <c r="H13" s="59"/>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -1388,7 +1436,7 @@
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="54" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -1401,14 +1449,14 @@
       <c r="E15" s="18">
         <v>1879</v>
       </c>
-      <c r="F15" s="18">
-        <v>1942</v>
+      <c r="F15" s="60" t="s">
+        <v>52</v>
       </c>
       <c r="G15" s="18"/>
-      <c r="H15" s="57"/>
+      <c r="H15" s="56"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="58"/>
+      <c r="A16" s="54"/>
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -1422,10 +1470,10 @@
         <v>12700</v>
       </c>
       <c r="F16" s="20"/>
-      <c r="H16" s="57"/>
+      <c r="H16" s="56"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="21" t="s">
         <v>28</v>
       </c>
@@ -1436,10 +1484,10 @@
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="34"/>
-      <c r="H17" s="57"/>
+      <c r="H17" s="56"/>
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="57" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
@@ -1456,10 +1504,10 @@
       </c>
       <c r="F18" s="28"/>
       <c r="G18" s="36"/>
-      <c r="H18" s="54"/>
+      <c r="H18" s="58"/>
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
+      <c r="A19" s="57"/>
       <c r="B19" t="s">
         <v>31</v>
       </c>
@@ -1470,10 +1518,10 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="37"/>
-      <c r="H19" s="54"/>
+      <c r="H19" s="58"/>
     </row>
     <row r="20" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="54" t="s">
         <v>32</v>
       </c>
       <c r="B20" t="s">
@@ -1486,10 +1534,10 @@
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="32"/>
-      <c r="H20" s="57"/>
+      <c r="H20" s="56"/>
     </row>
     <row r="21" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="21" t="s">
         <v>34</v>
       </c>
@@ -1500,7 +1548,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
       <c r="G21" s="34"/>
-      <c r="H21" s="57"/>
+      <c r="H21" s="56"/>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
@@ -1524,8 +1572,8 @@
       <c r="G22" s="38"/>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="55" t="s">
+    <row r="23" spans="1:8" s="3" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="57" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
@@ -1535,14 +1583,14 @@
       <c r="E23" s="28">
         <v>19210</v>
       </c>
-      <c r="F23" s="28">
-        <v>19201</v>
+      <c r="F23" s="62" t="s">
+        <v>53</v>
       </c>
       <c r="G23" s="36"/>
-      <c r="H23" s="54"/>
+      <c r="H23" s="58"/>
     </row>
     <row r="24" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="55"/>
+      <c r="A24" s="57"/>
       <c r="B24" t="s">
         <v>39</v>
       </c>
@@ -1550,10 +1598,10 @@
       <c r="E24" s="9">
         <v>79183</v>
       </c>
-      <c r="H24" s="54"/>
+      <c r="H24" s="58"/>
     </row>
     <row r="25" spans="1:8" s="4" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
+      <c r="A25" s="57"/>
       <c r="B25" s="40" t="s">
         <v>40</v>
       </c>
@@ -1562,7 +1610,7 @@
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
       <c r="G25" s="48"/>
-      <c r="H25" s="54"/>
+      <c r="H25" s="58"/>
     </row>
     <row r="26" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41"/>
@@ -1591,18 +1639,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="H7:H13"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="H18:H19"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A7:A13"/>
     <mergeCell ref="H20:H21"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="H7:H13"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="H18:H19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>

</xml_diff>

<commit_message>
add logic size in excel
</commit_message>
<xml_diff>
--- a/docs/smtcomp25_stats.xlsx
+++ b/docs/smtcomp25_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengyanglu/Desktop/z3alpha/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FADC08-59AF-C342-B97A-9589EB728896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EC09E0-8834-7149-81E9-DED8019D8388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-680" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Logics</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>NIA</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t xml:space="preserve">NRA </t>
@@ -494,7 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -647,32 +644,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1162,7 +1169,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1189,7 +1196,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>3</v>
@@ -1202,72 +1209,70 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="61" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="18"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="18">
+        <v>536</v>
+      </c>
       <c r="E2" s="18">
         <v>387</v>
       </c>
-      <c r="F2" s="60" t="s">
-        <v>43</v>
+      <c r="F2" s="54" t="s">
+        <v>42</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="59"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="54"/>
+      <c r="A3" s="61"/>
       <c r="B3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="20"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="20">
+        <v>2439</v>
+      </c>
       <c r="E3" s="20">
         <v>2177</v>
       </c>
-      <c r="F3" s="61" t="s">
-        <v>44</v>
+      <c r="F3" s="55" t="s">
+        <v>43</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="59"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="54"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>11</v>
-      </c>
+      <c r="C4" s="16"/>
       <c r="D4" s="20">
         <v>257</v>
       </c>
       <c r="E4" s="20">
         <v>210</v>
       </c>
-      <c r="F4" s="61" t="s">
-        <v>45</v>
+      <c r="F4" s="55" t="s">
+        <v>44</v>
       </c>
       <c r="G4" s="33"/>
       <c r="H4" s="59"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="22"/>
+        <v>11</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="22">
+        <v>3819</v>
+      </c>
       <c r="E5" s="22">
         <v>3810</v>
       </c>
@@ -1277,14 +1282,12 @@
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>8</v>
-      </c>
+      <c r="C6" s="24"/>
       <c r="D6" s="25">
         <v>6185</v>
       </c>
@@ -1296,118 +1299,113 @@
       <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="18"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="18">
+        <v>78</v>
+      </c>
       <c r="E7" s="18"/>
-      <c r="F7" s="60" t="s">
-        <v>46</v>
+      <c r="F7" s="54" t="s">
+        <v>45</v>
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="59"/>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="55"/>
-      <c r="B8" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="20"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="20">
+        <v>1567</v>
+      </c>
       <c r="E8" s="20">
         <v>1265</v>
       </c>
-      <c r="F8" s="61" t="s">
-        <v>47</v>
+      <c r="F8" s="55" t="s">
+        <v>46</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="59"/>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="55"/>
-      <c r="B9" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="20"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="20">
+        <v>3</v>
+      </c>
       <c r="E9" s="20"/>
-      <c r="F9" s="61" t="s">
-        <v>48</v>
+      <c r="F9" s="55" t="s">
+        <v>47</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="59"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="55"/>
-      <c r="B10" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="20"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="20">
+        <v>1480</v>
+      </c>
       <c r="E10" s="20">
         <v>1029</v>
       </c>
-      <c r="F10" s="61" t="s">
-        <v>49</v>
+      <c r="F10" s="55" t="s">
+        <v>48</v>
       </c>
       <c r="G10" s="33"/>
       <c r="H10" s="59"/>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="55"/>
-      <c r="B11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="20"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="20">
+        <v>1010</v>
+      </c>
       <c r="E11" s="20"/>
-      <c r="F11" s="61" t="s">
-        <v>50</v>
+      <c r="F11" s="55" t="s">
+        <v>49</v>
       </c>
       <c r="G11" s="33"/>
       <c r="H11" s="59"/>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="55"/>
-      <c r="B12" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="20"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="20">
+        <v>4424</v>
+      </c>
       <c r="E12" s="20">
         <v>3935</v>
       </c>
-      <c r="F12" s="61" t="s">
-        <v>51</v>
+      <c r="F12" s="55" t="s">
+        <v>50</v>
       </c>
       <c r="G12" s="33"/>
       <c r="H12" s="59"/>
     </row>
     <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="22"/>
+        <v>21</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="22">
+        <v>13532</v>
+      </c>
       <c r="E13" s="22">
         <v>6214</v>
       </c>
@@ -1417,51 +1415,46 @@
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>8</v>
-      </c>
+      <c r="C14" s="24"/>
       <c r="D14" s="24">
         <v>46191</v>
       </c>
       <c r="E14" s="51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="38"/>
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="18"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="18">
+        <v>2528</v>
+      </c>
       <c r="E15" s="18">
         <v>1879</v>
       </c>
-      <c r="F15" s="60" t="s">
-        <v>52</v>
+      <c r="F15" s="54" t="s">
+        <v>51</v>
       </c>
       <c r="G15" s="18"/>
-      <c r="H15" s="56"/>
+      <c r="H15" s="60"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="54"/>
+      <c r="A16" s="61"/>
       <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D16" s="20">
         <v>13306</v>
@@ -1470,32 +1463,30 @@
         <v>12700</v>
       </c>
       <c r="F16" s="20"/>
-      <c r="H16" s="56"/>
+      <c r="H16" s="60"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
+      <c r="A17" s="61"/>
       <c r="B17" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="22"/>
+        <v>27</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="22">
+        <v>7</v>
+      </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="34"/>
-      <c r="H17" s="56"/>
-    </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
+      <c r="H17" s="60"/>
+    </row>
+    <row r="18" spans="1:8" s="6" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>8</v>
-      </c>
+      <c r="C18" s="27"/>
       <c r="D18" s="28">
         <v>1753</v>
       </c>
@@ -1504,58 +1495,58 @@
       </c>
       <c r="F18" s="28"/>
       <c r="G18" s="36"/>
-      <c r="H18" s="58"/>
+      <c r="H18" s="57"/>
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57"/>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="30"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="30">
+        <v>255</v>
+      </c>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="37"/>
-      <c r="H19" s="58"/>
+      <c r="H19" s="57"/>
     </row>
     <row r="20" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="18"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="18">
+        <v>25452</v>
+      </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="32"/>
-      <c r="H20" s="56"/>
+      <c r="H20" s="60"/>
     </row>
     <row r="21" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="54"/>
-      <c r="B21" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="22"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="22">
+        <v>3</v>
+      </c>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
       <c r="G21" s="34"/>
-      <c r="H21" s="56"/>
+      <c r="H21" s="60"/>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
         <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
       </c>
       <c r="C22" s="24" t="s">
         <v>8</v>
@@ -1573,44 +1564,51 @@
       <c r="H22" s="24"/>
     </row>
     <row r="23" spans="1:8" s="3" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="28"/>
+      <c r="D23" s="24">
+        <v>22172</v>
+      </c>
       <c r="E23" s="28">
         <v>19210</v>
       </c>
-      <c r="F23" s="62" t="s">
-        <v>53</v>
+      <c r="F23" s="56" t="s">
+        <v>52</v>
       </c>
       <c r="G23" s="36"/>
-      <c r="H23" s="58"/>
+      <c r="H23" s="57"/>
     </row>
     <row r="24" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="57"/>
+      <c r="A24" s="58"/>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="27"/>
+      <c r="D24" s="9">
+        <v>84411</v>
+      </c>
       <c r="E24" s="9">
         <v>79183</v>
       </c>
-      <c r="H24" s="58"/>
+      <c r="H24" s="57"/>
     </row>
     <row r="25" spans="1:8" s="4" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="57"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="39"/>
-      <c r="D25" s="29"/>
+      <c r="D25" s="29">
+        <v>70</v>
+      </c>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
       <c r="G25" s="48"/>
-      <c r="H25" s="58"/>
+      <c r="H25" s="57"/>
     </row>
     <row r="26" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41"/>

</xml_diff>

<commit_message>
add qf_idl 4 core
</commit_message>
<xml_diff>
--- a/docs/smtcomp25_stats.xlsx
+++ b/docs/smtcomp25_stats.xlsx
@@ -113,13 +113,13 @@
     <t>UFDTNIA</t>
   </si>
   <si>
-    <t>978 [1 core]</t>
+    <t>978 [1 core], 986 [4 core]</t>
   </si>
   <si>
     <t>UFDTNIRA</t>
   </si>
   <si>
-    <t>3949 [1 core]</t>
+    <t>3949 [1 core], 3954 [4 core]</t>
   </si>
   <si>
     <t>UFNIA</t>
@@ -1781,11 +1781,11 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
Add qfs 4 core eval results
</commit_message>
<xml_diff>
--- a/docs/smtcomp25_stats.xlsx
+++ b/docs/smtcomp25_stats.xlsx
@@ -185,7 +185,7 @@
     <t>QF_S</t>
   </si>
   <si>
-    <t>19201 [1 core]</t>
+    <t>19201 [1 core], 19263 [4 core]</t>
   </si>
   <si>
     <t>QF_SLIA</t>
@@ -1781,11 +1781,11 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
add qfnia, ufnia, qfslia paral strats eval on reduced test size to excel
</commit_message>
<xml_diff>
--- a/docs/smtcomp25_stats.xlsx
+++ b/docs/smtcomp25_stats.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Logics</t>
   </si>
@@ -125,6 +125,9 @@
     <t>UFNIA</t>
   </si>
   <si>
+    <t>2483 [4core, 60s timeout, 5000 instances]</t>
+  </si>
+  <si>
     <t>QF_Bitvec</t>
   </si>
   <si>
@@ -167,6 +170,9 @@
     <t>QF_NIA</t>
   </si>
   <si>
+    <t>3968 [4core, 60s timeout, 5000 instances]</t>
+  </si>
+  <si>
     <t>QF_NIRA</t>
   </si>
   <si>
@@ -189,6 +195,9 @@
   </si>
   <si>
     <t>QF_SLIA</t>
+  </si>
+  <si>
+    <t>9418 [4core, 60s timeout, 10000 instances]</t>
   </si>
   <si>
     <t>QF_SNIA</t>
@@ -1781,11 +1790,11 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="7"/>
@@ -2027,23 +2036,25 @@
       <c r="E13" s="27">
         <v>6214</v>
       </c>
-      <c r="F13" s="27"/>
+      <c r="F13" s="27" t="s">
+        <v>32</v>
+      </c>
       <c r="G13" s="28"/>
       <c r="H13" s="21"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="17.1" spans="1:8">
       <c r="A14" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="30">
         <v>46191</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="39"/>
@@ -2051,10 +2062,10 @@
     </row>
     <row r="15" s="3" customFormat="1" ht="15.75" spans="1:8">
       <c r="A15" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="18">
@@ -2064,7 +2075,7 @@
         <v>1879</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="9"/>
@@ -2072,7 +2083,7 @@
     <row r="16" ht="15" spans="1:8">
       <c r="A16" s="15"/>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D16" s="21">
         <v>13306</v>
@@ -2086,7 +2097,7 @@
     <row r="17" ht="15.75" customHeight="1" spans="1:8">
       <c r="A17" s="15"/>
       <c r="B17" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="27">
@@ -2099,10 +2110,10 @@
     </row>
     <row r="18" s="4" customFormat="1" ht="17" customHeight="1" spans="1:8">
       <c r="A18" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="42"/>
       <c r="D18" s="43">
@@ -2112,7 +2123,7 @@
         <v>1588</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G18" s="45"/>
       <c r="H18" s="30"/>
@@ -2120,7 +2131,7 @@
     <row r="19" s="5" customFormat="1" ht="16.5" spans="1:8">
       <c r="A19" s="13"/>
       <c r="B19" s="46" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="48">
@@ -2133,24 +2144,26 @@
     </row>
     <row r="20" ht="15.75" spans="1:8">
       <c r="A20" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="18">
         <v>25452</v>
       </c>
       <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
+      <c r="F20" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="G20" s="20"/>
       <c r="H20" s="9"/>
     </row>
     <row r="21" ht="15.75" spans="1:8">
       <c r="A21" s="15"/>
       <c r="B21" s="50" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="27">
@@ -2163,13 +2176,13 @@
     </row>
     <row r="22" s="1" customFormat="1" ht="17.1" spans="1:8">
       <c r="A22" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D22" s="30">
         <v>12154</v>
@@ -2185,10 +2198,10 @@
     </row>
     <row r="23" s="6" customFormat="1" ht="16.5" spans="1:8">
       <c r="A23" s="13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D23" s="30">
         <v>22172</v>
@@ -2197,7 +2210,7 @@
         <v>19210</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G23" s="45"/>
       <c r="H23" s="30"/>
@@ -2205,7 +2218,7 @@
     <row r="24" ht="16.5" spans="1:8">
       <c r="A24" s="13"/>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C24" s="42"/>
       <c r="D24" s="9">
@@ -2214,12 +2227,15 @@
       <c r="E24" s="9">
         <v>79183</v>
       </c>
+      <c r="F24" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="H24" s="30"/>
     </row>
     <row r="25" s="5" customFormat="1" ht="16.5" spans="1:8">
       <c r="A25" s="13"/>
       <c r="B25" s="52" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C25" s="47"/>
       <c r="D25" s="53">
@@ -2227,7 +2243,7 @@
       </c>
       <c r="E25" s="53"/>
       <c r="F25" s="53" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G25" s="54"/>
       <c r="H25" s="30"/>

</xml_diff>

<commit_message>
add qf_lia paral strat eval results to excel and output files
</commit_message>
<xml_diff>
--- a/docs/smtcomp25_stats.xlsx
+++ b/docs/smtcomp25_stats.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Logics</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>QF_LIA</t>
+  </si>
+  <si>
+    <t>12625 [4 core]</t>
   </si>
   <si>
     <t>QF_LIRA</t>
@@ -1790,11 +1793,11 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="7"/>
@@ -2080,7 +2083,7 @@
       <c r="G15" s="18"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" ht="15" spans="1:8">
+    <row r="16" spans="1:8">
       <c r="A16" s="15"/>
       <c r="B16" t="s">
         <v>39</v>
@@ -2091,13 +2094,15 @@
       <c r="E16" s="41">
         <v>12700</v>
       </c>
-      <c r="F16" s="21"/>
+      <c r="F16" s="21" t="s">
+        <v>40</v>
+      </c>
       <c r="H16" s="9"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" spans="1:8">
       <c r="A17" s="15"/>
       <c r="B17" s="25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="27">
@@ -2110,10 +2115,10 @@
     </row>
     <row r="18" s="4" customFormat="1" ht="17" customHeight="1" spans="1:8">
       <c r="A18" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="42"/>
       <c r="D18" s="43">
@@ -2123,7 +2128,7 @@
         <v>1588</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G18" s="45"/>
       <c r="H18" s="30"/>
@@ -2131,7 +2136,7 @@
     <row r="19" s="5" customFormat="1" ht="16.5" spans="1:8">
       <c r="A19" s="13"/>
       <c r="B19" s="46" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="48">
@@ -2144,10 +2149,10 @@
     </row>
     <row r="20" ht="15.75" spans="1:8">
       <c r="A20" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="18">
@@ -2155,7 +2160,7 @@
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="9"/>
@@ -2163,7 +2168,7 @@
     <row r="21" ht="15.75" spans="1:8">
       <c r="A21" s="15"/>
       <c r="B21" s="50" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="27">
@@ -2176,13 +2181,13 @@
     </row>
     <row r="22" s="1" customFormat="1" ht="17.1" spans="1:8">
       <c r="A22" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D22" s="30">
         <v>12154</v>
@@ -2198,10 +2203,10 @@
     </row>
     <row r="23" s="6" customFormat="1" ht="16.5" spans="1:8">
       <c r="A23" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" s="30">
         <v>22172</v>
@@ -2210,7 +2215,7 @@
         <v>19210</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G23" s="45"/>
       <c r="H23" s="30"/>
@@ -2218,7 +2223,7 @@
     <row r="24" ht="16.5" spans="1:8">
       <c r="A24" s="13"/>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="42"/>
       <c r="D24" s="9">
@@ -2228,14 +2233,14 @@
         <v>79183</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H24" s="30"/>
     </row>
     <row r="25" s="5" customFormat="1" ht="16.5" spans="1:8">
       <c r="A25" s="13"/>
       <c r="B25" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C25" s="47"/>
       <c r="D25" s="53">
@@ -2243,7 +2248,7 @@
       </c>
       <c r="E25" s="53"/>
       <c r="F25" s="53" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G25" s="54"/>
       <c r="H25" s="30"/>

</xml_diff>

<commit_message>
update udftnia z3 default res in excel
</commit_message>
<xml_diff>
--- a/docs/smtcomp25_stats.xlsx
+++ b/docs/smtcomp25_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengyanglu/Desktop/z3alpha/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6972C9D-7B41-AD4B-B60B-81E92FEC74A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A461F0F-0F71-8D40-9EFB-4255D99F65DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2520" windowWidth="29400" windowHeight="17220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Division_summuary" sheetId="1" r:id="rId1"/>
@@ -512,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -596,12 +596,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -681,9 +675,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -711,9 +702,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -794,6 +782,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -812,10 +803,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1319,24 +1307,24 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="66" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="63" customWidth="1"/>
     <col min="3" max="3" width="24.5" style="12" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" style="12" customWidth="1"/>
     <col min="5" max="5" width="36.5" style="12" customWidth="1"/>
-    <col min="6" max="6" width="39" style="79" customWidth="1"/>
+    <col min="6" max="6" width="39" style="75" customWidth="1"/>
     <col min="7" max="7" width="91.5" style="13" customWidth="1"/>
     <col min="8" max="8" width="62.6640625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="54" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
@@ -1359,10 +1347,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="55" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -1374,15 +1362,15 @@
       <c r="E2" s="18">
         <v>387</v>
       </c>
-      <c r="F2" s="67">
+      <c r="F2" s="64">
         <v>435</v>
       </c>
       <c r="G2" s="19"/>
-      <c r="H2" s="102"/>
+      <c r="H2" s="99"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="105"/>
-      <c r="B3" s="58" t="s">
+      <c r="A3" s="102"/>
+      <c r="B3" s="56" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -1394,15 +1382,15 @@
       <c r="E3" s="21">
         <v>2177</v>
       </c>
-      <c r="F3" s="68">
+      <c r="F3" s="65">
         <v>2245</v>
       </c>
       <c r="G3" s="22"/>
-      <c r="H3" s="102"/>
+      <c r="H3" s="99"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="105"/>
-      <c r="B4" s="58" t="s">
+      <c r="A4" s="102"/>
+      <c r="B4" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="17"/>
@@ -1412,15 +1400,15 @@
       <c r="E4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="65" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="22"/>
-      <c r="H4" s="102"/>
+      <c r="H4" s="99"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="105"/>
-      <c r="B5" s="59" t="s">
+      <c r="A5" s="102"/>
+      <c r="B5" s="57" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="23" t="s">
@@ -1432,17 +1420,17 @@
       <c r="E5" s="24">
         <v>3810</v>
       </c>
-      <c r="F5" s="69">
+      <c r="F5" s="66">
         <v>3815</v>
       </c>
       <c r="G5" s="25"/>
-      <c r="H5" s="102"/>
+      <c r="H5" s="99"/>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="58" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="27"/>
@@ -1452,35 +1440,35 @@
       <c r="E6" s="28">
         <v>5585</v>
       </c>
-      <c r="F6" s="70"/>
+      <c r="F6" s="67"/>
       <c r="G6" s="29" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="99">
+      <c r="C7" s="94"/>
+      <c r="D7" s="95">
         <v>78</v>
       </c>
-      <c r="E7" s="99">
+      <c r="E7" s="95">
         <v>39</v>
       </c>
-      <c r="F7" s="100">
+      <c r="F7" s="96">
         <v>39</v>
       </c>
-      <c r="G7" s="107"/>
-      <c r="H7" s="102"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="99"/>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="106"/>
-      <c r="B8" s="61" t="s">
+      <c r="A8" s="103"/>
+      <c r="B8" s="59" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="20">
@@ -1489,29 +1477,28 @@
       <c r="E8" s="20">
         <v>1265</v>
       </c>
-      <c r="F8" s="71">
+      <c r="F8" s="68">
         <v>1267</v>
       </c>
       <c r="G8" s="31"/>
-      <c r="H8" s="102"/>
-    </row>
-    <row r="9" spans="1:8" s="113" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="106"/>
-      <c r="B9" s="108" t="s">
+      <c r="H8" s="99"/>
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="103"/>
+      <c r="B9" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="110">
+      <c r="D9" s="20">
         <v>3</v>
       </c>
-      <c r="E9" s="110"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="102"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="99"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="106"/>
-      <c r="B10" s="61" t="s">
+      <c r="A10" s="103"/>
+      <c r="B10" s="59" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="20">
@@ -1520,33 +1507,35 @@
       <c r="E10" s="20">
         <v>1029</v>
       </c>
-      <c r="F10" s="71">
+      <c r="F10" s="68">
         <v>1029</v>
       </c>
       <c r="G10" s="31"/>
-      <c r="H10" s="102"/>
-    </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="106"/>
-      <c r="B11" s="62" t="s">
+      <c r="H10" s="99"/>
+    </row>
+    <row r="11" spans="1:8" s="109" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="103"/>
+      <c r="B11" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33">
+      <c r="C11" s="105"/>
+      <c r="D11" s="106">
         <v>1010</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="72">
+      <c r="E11" s="106">
+        <v>988</v>
+      </c>
+      <c r="F11" s="107">
         <v>986</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="102"/>
+      <c r="H11" s="99"/>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="106"/>
-      <c r="B12" s="61" t="s">
+      <c r="A12" s="103"/>
+      <c r="B12" s="59" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="20">
@@ -1555,57 +1544,57 @@
       <c r="E12" s="20">
         <v>3935</v>
       </c>
-      <c r="F12" s="71">
+      <c r="F12" s="68">
         <v>3954</v>
       </c>
       <c r="G12" s="31"/>
-      <c r="H12" s="102"/>
+      <c r="H12" s="99"/>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="106"/>
-      <c r="B13" s="63" t="s">
+      <c r="A13" s="103"/>
+      <c r="B13" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="36">
+      <c r="C13" s="33"/>
+      <c r="D13" s="34">
         <v>13532</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="34">
         <v>6214</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="102"/>
+      <c r="H13" s="99"/>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="36" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="37">
         <v>46191</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="74"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="39"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" s="7" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="105" t="s">
+      <c r="A15" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="55" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -1617,111 +1606,111 @@
       <c r="E15" s="18">
         <v>1879</v>
       </c>
-      <c r="F15" s="67">
+      <c r="F15" s="64">
         <v>2087</v>
       </c>
       <c r="G15" s="18"/>
-      <c r="H15" s="103"/>
-    </row>
-    <row r="16" spans="1:8" s="80" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="105"/>
-      <c r="B16" s="91" t="s">
+      <c r="H15" s="100"/>
+    </row>
+    <row r="16" spans="1:8" s="76" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="102"/>
+      <c r="B16" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="92" t="s">
+      <c r="C16" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="93">
+      <c r="D16" s="89">
         <v>13306</v>
       </c>
-      <c r="E16" s="94" t="s">
+      <c r="E16" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="95" t="s">
+      <c r="F16" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="96" t="s">
+      <c r="G16" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="103"/>
+      <c r="H16" s="100"/>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="105"/>
-      <c r="B17" s="59" t="s">
+      <c r="A17" s="102"/>
+      <c r="B17" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="39" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="24">
         <v>7</v>
       </c>
       <c r="E17" s="24"/>
-      <c r="F17" s="69"/>
+      <c r="F17" s="66"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="103"/>
+      <c r="H17" s="100"/>
     </row>
     <row r="18" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="101" t="s">
+      <c r="A18" s="98" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="43">
+      <c r="C18" s="40"/>
+      <c r="D18" s="41">
         <v>1753</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="41">
         <v>1588</v>
       </c>
-      <c r="F18" s="75">
+      <c r="F18" s="71">
         <v>1632</v>
       </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="104"/>
-    </row>
-    <row r="19" spans="1:8" s="85" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="101"/>
-      <c r="B19" s="80" t="s">
+      <c r="G18" s="42"/>
+      <c r="H18" s="101"/>
+    </row>
+    <row r="19" spans="1:8" s="81" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="98"/>
+      <c r="B19" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="82">
+      <c r="D19" s="78">
         <v>255</v>
       </c>
-      <c r="E19" s="82"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="104"/>
-    </row>
-    <row r="20" spans="1:8" s="80" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="105" t="s">
+      <c r="E19" s="78"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="101"/>
+    </row>
+    <row r="20" spans="1:8" s="76" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="87">
+      <c r="D20" s="83">
         <v>25452</v>
       </c>
-      <c r="E20" s="88" t="s">
+      <c r="E20" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="89" t="s">
+      <c r="F20" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="90"/>
-      <c r="H20" s="103"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="100"/>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="105"/>
-      <c r="B21" s="59" t="s">
+      <c r="A21" s="102"/>
+      <c r="B21" s="57" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="23" t="s">
@@ -1731,34 +1720,34 @@
         <v>3</v>
       </c>
       <c r="E21" s="24"/>
-      <c r="F21" s="69"/>
+      <c r="F21" s="66"/>
       <c r="G21" s="25"/>
-      <c r="H21" s="103"/>
+      <c r="H21" s="100"/>
     </row>
     <row r="22" spans="1:8" s="6" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="36" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="37">
         <v>12154</v>
       </c>
-      <c r="E22" s="39">
+      <c r="E22" s="37">
         <v>11569</v>
       </c>
-      <c r="F22" s="74">
+      <c r="F22" s="70">
         <v>11676</v>
       </c>
-      <c r="G22" s="40"/>
-      <c r="H22" s="39"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="37"/>
     </row>
     <row r="23" spans="1:8" s="9" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="101" t="s">
+      <c r="A23" s="98" t="s">
         <v>47</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1767,20 +1756,20 @@
       <c r="C23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="39">
+      <c r="D23" s="37">
         <v>22172</v>
       </c>
-      <c r="E23" s="43">
+      <c r="E23" s="41">
         <v>19210</v>
       </c>
-      <c r="F23" s="75">
+      <c r="F23" s="71">
         <v>19263</v>
       </c>
-      <c r="G23" s="44"/>
-      <c r="H23" s="104"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="101"/>
     </row>
     <row r="24" spans="1:8" s="4" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="101"/>
+      <c r="A24" s="98"/>
       <c r="B24" s="4" t="s">
         <v>49</v>
       </c>
@@ -1793,56 +1782,56 @@
       <c r="E24" s="32">
         <v>79183</v>
       </c>
-      <c r="F24" s="76" t="s">
+      <c r="F24" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="37" t="s">
+      <c r="G24" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="H24" s="104"/>
+      <c r="H24" s="101"/>
     </row>
     <row r="25" spans="1:8" s="10" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="101"/>
-      <c r="B25" s="64" t="s">
+      <c r="A25" s="98"/>
+      <c r="B25" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="46">
+      <c r="D25" s="44">
         <v>70</v>
       </c>
-      <c r="E25" s="46"/>
-      <c r="F25" s="77">
+      <c r="E25" s="44"/>
+      <c r="F25" s="73">
         <v>70</v>
       </c>
-      <c r="G25" s="47"/>
-      <c r="H25" s="104"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="101"/>
     </row>
     <row r="26" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="48"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="51"/>
+      <c r="A27" s="49"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="52"/>
+      <c r="A28" s="50"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="53"/>
+      <c r="A29" s="51"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="54"/>
+      <c r="A30" s="52"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="55"/>
+      <c r="A31" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
update excel with qf_slia results
</commit_message>
<xml_diff>
--- a/docs/smtcomp25_stats.xlsx
+++ b/docs/smtcomp25_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengyanglu/Desktop/z3alpha/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D24571-79BE-D048-BF55-2058C0A21503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3959570-C1D4-9140-B702-6188FF8CF7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1860" windowWidth="29400" windowHeight="17220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Division_summuary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Logics</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>QF_SLIA</t>
-  </si>
-  <si>
-    <t>9418 [4core, 60s timeout, 10000 instances]</t>
   </si>
   <si>
     <t>QF_SNIA</t>
@@ -171,6 +168,12 @@
   </si>
   <si>
     <t>Yes [P]</t>
+  </si>
+  <si>
+    <t>9418 [60s timeout, 10000 instances]</t>
+  </si>
+  <si>
+    <t>9189 [60s timeout, 10000 instances]</t>
   </si>
 </sst>
 </file>
@@ -458,13 +461,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -517,15 +519,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,9 +609,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -689,6 +679,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1177,387 +1176,391 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="51" customWidth="1"/>
-    <col min="3" max="3" width="24.5" style="11" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="36.5" style="11" customWidth="1"/>
-    <col min="6" max="6" width="39" style="60" customWidth="1"/>
-    <col min="7" max="7" width="91.5" style="12" customWidth="1"/>
-    <col min="8" max="8" width="62.6640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="47" customWidth="1"/>
+    <col min="3" max="3" width="24.5" style="10" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="36.5" style="10" customWidth="1"/>
+    <col min="6" max="6" width="39" style="55" customWidth="1"/>
+    <col min="7" max="7" width="91.5" style="11" customWidth="1"/>
+    <col min="8" max="8" width="62.6640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13"/>
-      <c r="B1" s="45" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <v>536</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <v>387</v>
       </c>
-      <c r="F2" s="52">
+      <c r="F2" s="48">
         <v>435</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="79"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="82"/>
-      <c r="B3" s="47" t="s">
+      <c r="A3" s="77"/>
+      <c r="B3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="18">
         <v>2439</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="18">
         <v>2177</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="49">
         <v>2245</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="79"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="82"/>
-      <c r="B4" s="47" t="s">
+      <c r="A4" s="77"/>
+      <c r="B4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="19">
+      <c r="C4" s="15"/>
+      <c r="D4" s="18">
         <v>257</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="79"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="74"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="82"/>
-      <c r="B5" s="48" t="s">
+      <c r="A5" s="77"/>
+      <c r="B5" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>3819</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="21">
         <v>3810</v>
       </c>
-      <c r="F5" s="54">
+      <c r="F5" s="50">
         <v>3815</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="79"/>
-    </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="74"/>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="24">
         <v>46191</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="55"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="28"/>
-    </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="82" t="s">
+      <c r="F6" s="51"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:8" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>2528</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>1879</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="48">
         <v>2087</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="80"/>
-    </row>
-    <row r="8" spans="1:8" s="61" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="82"/>
-      <c r="B8" s="72" t="s">
+      <c r="G7" s="16"/>
+      <c r="H7" s="75"/>
+    </row>
+    <row r="8" spans="1:8" s="56" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="77"/>
+      <c r="B8" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="69">
+        <v>13306</v>
+      </c>
+      <c r="E8" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="75"/>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="77"/>
+      <c r="B9" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="21">
+        <v>7</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="75"/>
+    </row>
+    <row r="10" spans="1:8" s="6" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28">
+        <v>1753</v>
+      </c>
+      <c r="E10" s="28">
+        <v>1588</v>
+      </c>
+      <c r="F10" s="52">
+        <v>1632</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10" s="76"/>
+    </row>
+    <row r="11" spans="1:8" s="61" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="73"/>
+      <c r="B11" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="58">
+        <v>255</v>
+      </c>
+      <c r="E11" s="58">
+        <v>205</v>
+      </c>
+      <c r="F11" s="59">
+        <v>203</v>
+      </c>
+      <c r="G11" s="60"/>
+      <c r="H11" s="76"/>
+    </row>
+    <row r="12" spans="1:8" s="56" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="63">
+        <v>25452</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="66"/>
+      <c r="H12" s="75"/>
+    </row>
+    <row r="13" spans="1:8" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="77"/>
+      <c r="B13" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="21">
+        <v>3</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="75"/>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="24">
+        <v>12154</v>
+      </c>
+      <c r="E14" s="24">
+        <v>11569</v>
+      </c>
+      <c r="F14" s="51">
+        <v>11676</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8" s="7" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="24">
+        <v>22172</v>
+      </c>
+      <c r="E15" s="28">
+        <v>19210</v>
+      </c>
+      <c r="F15" s="52">
+        <v>19263</v>
+      </c>
+      <c r="G15" s="29"/>
+      <c r="H15" s="76"/>
+    </row>
+    <row r="16" spans="1:8" s="56" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="73"/>
+      <c r="B16" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="79">
+        <v>84411</v>
+      </c>
+      <c r="E16" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="74">
-        <v>13306</v>
-      </c>
-      <c r="E8" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="76" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="80"/>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="82"/>
-      <c r="B9" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="30" t="s">
+      <c r="G16" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="76"/>
+    </row>
+    <row r="17" spans="1:8" s="8" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="73"/>
+      <c r="B17" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="22">
-        <v>7</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="80"/>
-    </row>
-    <row r="10" spans="1:8" s="7" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="78" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32">
-        <v>1753</v>
-      </c>
-      <c r="E10" s="32">
-        <v>1588</v>
-      </c>
-      <c r="F10" s="56">
-        <v>1632</v>
-      </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="81"/>
-    </row>
-    <row r="11" spans="1:8" s="66" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="78"/>
-      <c r="B11" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="63">
-        <v>255</v>
-      </c>
-      <c r="E11" s="63"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="81"/>
-    </row>
-    <row r="12" spans="1:8" s="61" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="82" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="68">
-        <v>25452</v>
-      </c>
-      <c r="E12" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="71"/>
-      <c r="H12" s="80"/>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="82"/>
-      <c r="B13" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="22">
-        <v>3</v>
-      </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="80"/>
-    </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="28">
-        <v>12154</v>
-      </c>
-      <c r="E14" s="28">
-        <v>11569</v>
-      </c>
-      <c r="F14" s="55">
-        <v>11676</v>
-      </c>
-      <c r="G14" s="29"/>
-      <c r="H14" s="28"/>
-    </row>
-    <row r="15" spans="1:8" s="8" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="78" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="28">
-        <v>22172</v>
-      </c>
-      <c r="E15" s="32">
-        <v>19210</v>
-      </c>
-      <c r="F15" s="56">
-        <v>19263</v>
-      </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="81"/>
-    </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
-      <c r="B16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="25">
-        <v>84411</v>
-      </c>
-      <c r="E16" s="25">
-        <v>79183</v>
-      </c>
-      <c r="F16" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="81"/>
-    </row>
-    <row r="17" spans="1:8" s="9" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
-      <c r="B17" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="35">
+      <c r="D17" s="31">
         <v>70</v>
       </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="58">
+      <c r="E17" s="31"/>
+      <c r="F17" s="53">
         <v>70</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="81"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="76"/>
     </row>
     <row r="18" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="40"/>
+      <c r="A19" s="36"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="41"/>
+      <c r="A20" s="37"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="38"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="43"/>
+      <c r="A22" s="39"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>